<commit_message>
commiting with  the latest code
</commit_message>
<xml_diff>
--- a/TestData/PAtestData.xlsx
+++ b/TestData/PAtestData.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Recordings" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Logout" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
   <si>
     <t xml:space="preserve">testNameDetails</t>
   </si>
@@ -560,7 +561,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -738,8 +739,8 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -824,4 +825,79 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.28"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="thejaswini+devscribe@navadhiti.com"/>
+    <hyperlink ref="E2" r:id="rId2" display="Teju@5555"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
commiting with methodmatcher exception in the TC_002
</commit_message>
<xml_diff>
--- a/TestData/PAtestData.xlsx
+++ b/TestData/PAtestData.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Recordings" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Logout" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Keyword" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
   <si>
     <t xml:space="preserve">testNameDetails</t>
   </si>
@@ -96,32 +97,33 @@
     <t xml:space="preserve">DoctorName</t>
   </si>
   <si>
-    <t xml:space="preserve">Filestatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rec code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validate login feature with valid credentials and filestatus</t>
+    <t xml:space="preserve">Targetdates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate login feature with valid credentials and filestatus Flow</t>
   </si>
   <si>
     <t xml:space="preserve">Teju two</t>
   </si>
   <si>
-    <t xml:space="preserve">scribe review pending</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REC-1782</t>
+    <t xml:space="preserve">`27/09/2024`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate login feature with valid credentials and no recordings </t>
+  </si>
+  <si>
+    <t xml:space="preserve">`01/01/2022`</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="d\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -185,7 +187,7 @@
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Monospace"/>
+      <name val="Ubuntu"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -194,15 +196,7 @@
       <u val="single"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Monospace"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Ubuntu"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -256,7 +250,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -290,23 +284,27 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -737,24 +735,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="56.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="65.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="30.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.44"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -764,13 +762,13 @@
       <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -779,43 +777,71 @@
       <c r="H1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+    </row>
+    <row r="2" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="H2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+    </row>
+    <row r="3" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="12" t="s">
+      <c r="G3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>29</v>
       </c>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="thejaswini+devscribe@navadhiti.com"/>
     <hyperlink ref="E2" r:id="rId2" display="Teju@5555"/>
+    <hyperlink ref="D3" r:id="rId3" display="thejaswini+devscribe@navadhiti.com"/>
+    <hyperlink ref="E3" r:id="rId4" display="Teju@5555"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -834,17 +860,91 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="36.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.28"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="thejaswini+devscribe@navadhiti.com"/>
+    <hyperlink ref="E2" r:id="rId2" display="Teju@5555"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="36.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
commiting with the page_005 and TC_005
</commit_message>
<xml_diff>
--- a/TestData/PAtestData.xlsx
+++ b/TestData/PAtestData.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Recordings" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Logout" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Keyword" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Recordingfile" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="47">
   <si>
     <t xml:space="preserve">testNameDetails</t>
   </si>
@@ -97,33 +98,83 @@
     <t xml:space="preserve">DoctorName</t>
   </si>
   <si>
-    <t xml:space="preserve">Targetdates</t>
-  </si>
-  <si>
     <t xml:space="preserve">Validate login feature with valid credentials and filestatus Flow</t>
   </si>
   <si>
     <t xml:space="preserve">Teju two</t>
   </si>
   <si>
-    <t xml:space="preserve">`27/09/2024`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validate login feature with valid credentials and no recordings </t>
-  </si>
-  <si>
-    <t xml:space="preserve">`01/01/2022`</t>
+    <t xml:space="preserve">keywordtext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instructiontext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add keyword with valid data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow the instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add keyword with existed data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OBGYN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add keyword with empty keyword as data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emptykeyword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,mnbvc*&amp;^%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add keyword with empty instruction as data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emptyinstruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kljhgfd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add keyword with spaces as data in keyword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keywordlimit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">,mnbvcx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add keyword with spaces as data in instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instructionlimit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zczxvcxcv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate recording file page with all functionalities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="d\ mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -200,6 +251,21 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF6A3E3E"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +316,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -291,20 +357,36 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -559,7 +641,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -735,10 +817,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -749,10 +831,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.44"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -774,74 +855,43 @@
       <c r="G1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="10" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-    </row>
-    <row r="2" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="B2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0"/>
-    </row>
-    <row r="3" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="thejaswini+devscribe@navadhiti.com"/>
     <hyperlink ref="E2" r:id="rId2" display="Teju@5555"/>
-    <hyperlink ref="D3" r:id="rId3" display="thejaswini+devscribe@navadhiti.com"/>
-    <hyperlink ref="E3" r:id="rId4" display="Teju@5555"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -933,58 +983,293 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="47.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="36.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="thejaswini+devscribe@navadhiti.com"/>
+    <hyperlink ref="E2" r:id="rId2" display="Teju@5555"/>
+    <hyperlink ref="D3" r:id="rId3" display="thejaswini+devscribe@navadhiti.com"/>
+    <hyperlink ref="E3" r:id="rId4" display="Teju@5555"/>
+    <hyperlink ref="D4" r:id="rId5" display="thejaswini+devscribe@navadhiti.com"/>
+    <hyperlink ref="E4" r:id="rId6" display="Teju@5555"/>
+    <hyperlink ref="D5" r:id="rId7" display="thejaswini+devscribe@navadhiti.com"/>
+    <hyperlink ref="E5" r:id="rId8" display="Teju@5555"/>
+    <hyperlink ref="D6" r:id="rId9" display="thejaswini+devscribe@navadhiti.com"/>
+    <hyperlink ref="E6" r:id="rId10" display="Teju@5555"/>
+    <hyperlink ref="D7" r:id="rId11" display="thejaswini+devscribe@navadhiti.com"/>
+    <hyperlink ref="E7" r:id="rId12" display="Teju@5555"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="72.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.2"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>